<commit_message>
refactoring Master class so default is project names are taken from latest master data set being provided. check_baselines() function added
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_4_2018.xlsx
+++ b/tests/resources/cut_down_master_4_2018.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="55">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -459,11 +459,11 @@
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -740,7 +740,9 @@
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">

</xml_diff>